<commit_message>
Poprawiam populacje bo sie zjebalo cos
</commit_message>
<xml_diff>
--- a/Populacja.xlsx
+++ b/Populacja.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20373"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\micha\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Michał\Desktop\Pakiety\ProjektPakiety\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E69B354E-0165-4C2C-BBBA-D0AECF2478D3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{600C246B-2B02-47E2-ABBC-DE60EA410CFE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{9E65CF9B-3397-4A09-B8E6-0FDCDE6970F2}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{9E65CF9B-3397-4A09-B8E6-0FDCDE6970F2}"/>
   </bookViews>
   <sheets>
-    <sheet name="Arkusz1" sheetId="1" r:id="rId1"/>
+    <sheet name="1" sheetId="1" r:id="rId1"/>
+    <sheet name="2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="4">
   <si>
     <t>Rok</t>
   </si>
@@ -35,12 +36,23 @@
   <si>
     <t xml:space="preserve">Różnica </t>
   </si>
+  <si>
+    <t>Procentowo</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -67,17 +79,23 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normalny" xfId="0" builtinId="0"/>
+    <cellStyle name="Procentowy" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -88,6 +106,34 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{519BEEFA-84FD-4D37-8170-C535834B4045}" name="Tabela3" displayName="Tabela3" ref="A1:D11" totalsRowShown="0">
+  <autoFilter ref="A1:D11" xr:uid="{519BEEFA-84FD-4D37-8170-C535834B4045}"/>
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{5D233DE0-9137-47C4-8462-5C725B96CAB2}" name="Rok"/>
+    <tableColumn id="2" xr3:uid="{C95BC123-DB86-4137-9701-D1785FAA58B7}" name="Liczba Żubrów"/>
+    <tableColumn id="3" xr3:uid="{5FD87E81-412A-49B2-8DAE-1FD17EB6BD62}" name="Różnica ">
+      <calculatedColumnFormula>B2-B1</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="4" xr3:uid="{72107978-7F8A-451E-A353-D9E999824099}" name="Procentowo" dataDxfId="0">
+      <calculatedColumnFormula>(Tabela3[[#This Row],[Różnica ]]/Tabela3[[#This Row],[Liczba Żubrów]])*100%</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{133CEDC6-0BF9-45FC-967E-E9D6CDDDF896}" name="Tabela4" displayName="Tabela4" ref="A1:B7" totalsRowShown="0">
+  <autoFilter ref="A1:B7" xr:uid="{133CEDC6-0BF9-45FC-967E-E9D6CDDDF896}"/>
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{55D6592F-D394-429D-9C94-083CDA76E6A8}" name="Rok"/>
+    <tableColumn id="2" xr3:uid="{BB114A4F-1C56-49EB-B4A0-15EA69A7C177}" name="Liczba Żubrów"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -387,19 +433,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F9B3A422-8057-4CCF-8EC9-C07E401C29D0}">
-  <dimension ref="A1:F11"/>
+  <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="14" customWidth="1"/>
-    <col min="6" max="6" width="13.42578125" customWidth="1"/>
+    <col min="2" max="2" width="15.5703125" customWidth="1"/>
+    <col min="3" max="3" width="10.28515625" customWidth="1"/>
+    <col min="6" max="6" width="15.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -409,14 +456,11 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" t="s">
-        <v>0</v>
-      </c>
-      <c r="F1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>2013</v>
       </c>
@@ -424,14 +468,12 @@
         <f>7+40+2+3+3+10+14+2+6+1+5+6+11+25+3+46+6+21+4+5+3+4+5+4+3+270+505+103+128</f>
         <v>1245</v>
       </c>
-      <c r="E2">
-        <v>1959</v>
-      </c>
-      <c r="F2">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D2">
+        <f>(Tabela3[[#This Row],[Różnica ]]/Tabela3[[#This Row],[Liczba Żubrów]])*100%</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2014</v>
       </c>
@@ -443,15 +485,12 @@
         <f>B3-B2</f>
         <v>174</v>
       </c>
-      <c r="E3">
-        <v>1970</v>
-      </c>
-      <c r="F3">
-        <f>31+2+9+3+2+3+14+2+28+16+2+3+38+197+7</f>
-        <v>357</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D3" s="1">
+        <f>(Tabela3[[#This Row],[Różnica ]]/Tabela3[[#This Row],[Liczba Żubrów]])*100%</f>
+        <v>0.1226215644820296</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2015</v>
       </c>
@@ -463,15 +502,12 @@
         <f t="shared" ref="C4:C11" si="0">B4-B3</f>
         <v>137</v>
       </c>
-      <c r="E4">
-        <v>1980</v>
-      </c>
-      <c r="F4">
-        <f>34+3+12+2+1+4+8+4+6+4+2+2+8+14+5+34+2+15+3+3+105+230+55+9</f>
-        <v>565</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D4" s="1">
+        <f>(Tabela3[[#This Row],[Różnica ]]/Tabela3[[#This Row],[Liczba Żubrów]])*100%</f>
+        <v>8.804627249357326E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>2016</v>
       </c>
@@ -483,15 +519,12 @@
         <f t="shared" si="0"/>
         <v>142</v>
       </c>
-      <c r="E5">
-        <v>1990</v>
-      </c>
-      <c r="F5">
-        <f>32+2+6+3+9+1+2+1+1+4+4+19+4+33+10+4+2+97+13+272+66+14</f>
-        <v>599</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D5" s="1">
+        <f>(Tabela3[[#This Row],[Różnica ]]/Tabela3[[#This Row],[Liczba Żubrów]])*100%</f>
+        <v>8.3627797408716134E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>2017</v>
       </c>
@@ -503,15 +536,12 @@
         <f t="shared" si="0"/>
         <v>175</v>
       </c>
-      <c r="E6">
-        <v>2000</v>
-      </c>
-      <c r="F6">
-        <f>37+2+4+6+10+2+3+2+5+9+25+3+28+25+2+6+140+26+306+60+16</f>
-        <v>717</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D6" s="1">
+        <f>(Tabela3[[#This Row],[Różnica ]]/Tabela3[[#This Row],[Liczba Żubrów]])*100%</f>
+        <v>9.3432995194874538E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>2018</v>
       </c>
@@ -523,15 +553,12 @@
         <f t="shared" si="0"/>
         <v>-53</v>
       </c>
-      <c r="E7" s="1">
-        <v>2010</v>
-      </c>
-      <c r="F7">
-        <f>43+2+5+2+8+7+4+4+1+3+5+26+2+42+6+17+2+4+5+3+304+473+91+94+81</f>
-        <v>1234</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D7" s="1">
+        <f>(Tabela3[[#This Row],[Różnica ]]/Tabela3[[#This Row],[Liczba Żubrów]])*100%</f>
+        <v>-2.9120879120879122E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>2019</v>
       </c>
@@ -543,8 +570,12 @@
         <f t="shared" si="0"/>
         <v>449</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D8" s="1">
+        <f>(Tabela3[[#This Row],[Różnica ]]/Tabela3[[#This Row],[Liczba Żubrów]])*100%</f>
+        <v>0.19788453063023359</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>2020</v>
       </c>
@@ -556,8 +587,12 @@
         <f t="shared" si="0"/>
         <v>54</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D9" s="1">
+        <f>(Tabela3[[#This Row],[Różnica ]]/Tabela3[[#This Row],[Liczba Żubrów]])*100%</f>
+        <v>2.3245802841153681E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>2021</v>
       </c>
@@ -569,8 +604,12 @@
         <f t="shared" si="0"/>
         <v>106</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D10" s="1">
+        <f>(Tabela3[[#This Row],[Różnica ]]/Tabela3[[#This Row],[Liczba Żubrów]])*100%</f>
+        <v>4.3639357760395223E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>2022</v>
       </c>
@@ -581,9 +620,95 @@
         <f t="shared" si="0"/>
         <v>174</v>
       </c>
+      <c r="D11" s="1">
+        <f>(Tabela3[[#This Row],[Różnica ]]/Tabela3[[#This Row],[Liczba Żubrów]])*100%</f>
+        <v>6.684594698424895E-2</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{08694621-01AC-45A8-A2E8-8CAA484C8E0E}">
+  <dimension ref="A1:B7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1959</v>
+      </c>
+      <c r="B2">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>1970</v>
+      </c>
+      <c r="B3">
+        <f>31+2+9+3+2+3+14+2+28+16+2+3+38+197+7</f>
+        <v>357</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>1980</v>
+      </c>
+      <c r="B4">
+        <f>34+3+12+2+1+4+8+4+6+4+2+2+8+14+5+34+2+15+3+3+105+230+55+9</f>
+        <v>565</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>1990</v>
+      </c>
+      <c r="B5">
+        <f>32+2+6+3+9+1+2+1+1+4+4+19+4+33+10+4+2+97+13+272+66+14</f>
+        <v>599</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>2000</v>
+      </c>
+      <c r="B6">
+        <f>37+2+4+6+10+2+3+2+5+9+25+3+28+25+2+6+140+26+306+60+16</f>
+        <v>717</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>2010</v>
+      </c>
+      <c r="B7">
+        <f>43+2+5+2+8+7+4+4+1+3+5+26+2+42+6+17+2+4+5+3+304+473+91+94+81</f>
+        <v>1234</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Ostateczna wersja 1 prezki v1
</commit_message>
<xml_diff>
--- a/Populacja.xlsx
+++ b/Populacja.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Michał\Desktop\Pakiety\ProjektPakiety\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{600C246B-2B02-47E2-ABBC-DE60EA410CFE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99437EAC-EE92-437C-9458-F5EFF4E36826}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{9E65CF9B-3397-4A09-B8E6-0FDCDE6970F2}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{9E65CF9B-3397-4A09-B8E6-0FDCDE6970F2}"/>
   </bookViews>
   <sheets>
     <sheet name="1" sheetId="1" r:id="rId1"/>
     <sheet name="2" sheetId="2" r:id="rId2"/>
+    <sheet name="3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="4">
   <si>
     <t>Rok</t>
   </si>
@@ -91,7 +92,10 @@
     <cellStyle name="Normalny" xfId="0" builtinId="0"/>
     <cellStyle name="Procentowy" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="2">
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
@@ -117,7 +121,7 @@
     <tableColumn id="3" xr3:uid="{5FD87E81-412A-49B2-8DAE-1FD17EB6BD62}" name="Różnica ">
       <calculatedColumnFormula>B2-B1</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{72107978-7F8A-451E-A353-D9E999824099}" name="Procentowo" dataDxfId="0">
+    <tableColumn id="4" xr3:uid="{72107978-7F8A-451E-A353-D9E999824099}" name="Procentowo" dataDxfId="1">
       <calculatedColumnFormula>(Tabela3[[#This Row],[Różnica ]]/Tabela3[[#This Row],[Liczba Żubrów]])*100%</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -131,6 +135,23 @@
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{55D6592F-D394-429D-9C94-083CDA76E6A8}" name="Rok"/>
     <tableColumn id="2" xr3:uid="{BB114A4F-1C56-49EB-B4A0-15EA69A7C177}" name="Liczba Żubrów"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{C5685D82-41ED-43A7-BF51-B3364622FC0F}" name="Tabela32" displayName="Tabela32" ref="A1:D11" totalsRowShown="0">
+  <autoFilter ref="A1:D11" xr:uid="{C5685D82-41ED-43A7-BF51-B3364622FC0F}"/>
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{DC57C2C8-9251-49AF-9390-BA38397C4314}" name="Rok"/>
+    <tableColumn id="2" xr3:uid="{28DB04E9-FBF4-48CC-A1A2-39E94BD1D431}" name="Liczba Żubrów"/>
+    <tableColumn id="3" xr3:uid="{B8B234E7-F8B4-43E0-B94C-0E9A2E85FF1C}" name="Różnica ">
+      <calculatedColumnFormula>B2-B1</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="4" xr3:uid="{A2DB2C59-0D35-4723-8253-97F510324DE0}" name="Procentowo" dataDxfId="0">
+      <calculatedColumnFormula>(Tabela32[[#This Row],[Różnica ]]/Tabela32[[#This Row],[Liczba Żubrów]])*100%</calculatedColumnFormula>
+    </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -435,8 +456,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F9B3A422-8057-4CCF-8EC9-C07E401C29D0}">
   <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -711,4 +732,201 @@
     <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FDE21DE9-5625-4254-9734-3F77F5BFA5B7}">
+  <dimension ref="A1:D11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>2013</v>
+      </c>
+      <c r="B2">
+        <f>7+40+2+3+3+10+14+2+6+1+5+6+11+25+3+46+6+21+4+5+3+4+5+4+3+270+505+103+128</f>
+        <v>1245</v>
+      </c>
+      <c r="D2">
+        <f>(Tabela32[[#This Row],[Różnica ]]/Tabela32[[#This Row],[Liczba Żubrów]])*100%</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2014</v>
+      </c>
+      <c r="B3">
+        <f>9+37+2+3+3+11+5+2+6+3+4+5+10+22+2+41+6+15+4+5+1+4+5+4+301+522+105+123+159</f>
+        <v>1419</v>
+      </c>
+      <c r="C3">
+        <f>B3-B2</f>
+        <v>174</v>
+      </c>
+      <c r="D3" s="1">
+        <f>(Tabela32[[#This Row],[Różnica ]]/Tabela32[[#This Row],[Liczba Żubrów]])*100%</f>
+        <v>0.1226215644820296</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>2015</v>
+      </c>
+      <c r="B4">
+        <f>8+28+2+3+3+10+11+6+4+6+3+7+12+27+2+43+8+7+1+4+6+4+4+344+578+107+134+184</f>
+        <v>1556</v>
+      </c>
+      <c r="C4">
+        <f t="shared" ref="C4:C11" si="0">B4-B3</f>
+        <v>137</v>
+      </c>
+      <c r="D4" s="1">
+        <f>(Tabela32[[#This Row],[Różnica ]]/Tabela32[[#This Row],[Liczba Żubrów]])*100%</f>
+        <v>8.804627249357326E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>2016</v>
+      </c>
+      <c r="B5">
+        <f>9+39+2+3+3+12+12+9+4+7+1+8+16+26+2+50+7+6+4+8+1+4+5+5+402+596+108+144+205</f>
+        <v>1698</v>
+      </c>
+      <c r="C5">
+        <f t="shared" si="0"/>
+        <v>142</v>
+      </c>
+      <c r="D5" s="1">
+        <f>(Tabela32[[#This Row],[Różnica ]]/Tabela32[[#This Row],[Liczba Żubrów]])*100%</f>
+        <v>8.3627797408716134E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>2017</v>
+      </c>
+      <c r="B6">
+        <f>8+43+1+3+4+13+10+8+4+8+9+11+27+3+42+7+6+4+9+1+5+7+5+487+654+120+158+216</f>
+        <v>1873</v>
+      </c>
+      <c r="C6">
+        <f t="shared" si="0"/>
+        <v>175</v>
+      </c>
+      <c r="D6" s="1">
+        <f>(Tabela32[[#This Row],[Różnica ]]/Tabela32[[#This Row],[Liczba Żubrów]])*100%</f>
+        <v>9.3432995194874538E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>2018</v>
+      </c>
+      <c r="B7">
+        <f>8+19+1+4+4+12+7+9+3+8+9+11+23+5+48+6+4+10+1+3+6+6+551+8+519+112+158+265+230</f>
+        <v>2050</v>
+      </c>
+      <c r="C7">
+        <f t="shared" si="0"/>
+        <v>177</v>
+      </c>
+      <c r="D7" s="1">
+        <f>(Tabela32[[#This Row],[Różnica ]]/Tabela32[[#This Row],[Liczba Żubrów]])*100%</f>
+        <v>8.634146341463414E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>2019</v>
+      </c>
+      <c r="B8">
+        <f>8+27+1+4+5+13+5+10+3+6+6+9+22+5+56+7+4+7+1+3+8+5+6+668+9+770+112+184+305</f>
+        <v>2269</v>
+      </c>
+      <c r="C8">
+        <f t="shared" si="0"/>
+        <v>219</v>
+      </c>
+      <c r="D8" s="1">
+        <f>(Tabela32[[#This Row],[Różnica ]]/Tabela32[[#This Row],[Liczba Żubrów]])*100%</f>
+        <v>9.6518289995592768E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>2020</v>
+      </c>
+      <c r="B9">
+        <f>6+31+1+11+3+4+5+6+7+3+4+8+13+19+6+45+5+7+4+7+5+3+7+6+3+707+17+715+117+214+334</f>
+        <v>2323</v>
+      </c>
+      <c r="C9">
+        <f t="shared" si="0"/>
+        <v>54</v>
+      </c>
+      <c r="D9" s="1">
+        <f>(Tabela32[[#This Row],[Różnica ]]/Tabela32[[#This Row],[Liczba Żubrów]])*100%</f>
+        <v>2.3245802841153681E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>2021</v>
+      </c>
+      <c r="B10">
+        <f>7+28+1+4+4+7+7+9+3+8+10+16+7+50+6+6+7+3+2+9+8+4+729+9+20+779+125+212+9+340</f>
+        <v>2429</v>
+      </c>
+      <c r="C10">
+        <f t="shared" si="0"/>
+        <v>106</v>
+      </c>
+      <c r="D10" s="1">
+        <f>(Tabela32[[#This Row],[Różnica ]]/Tabela32[[#This Row],[Liczba Żubrów]])*100%</f>
+        <v>4.3639357760395223E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>2022</v>
+      </c>
+      <c r="B11">
+        <v>2603</v>
+      </c>
+      <c r="C11">
+        <f t="shared" si="0"/>
+        <v>174</v>
+      </c>
+      <c r="D11" s="1">
+        <f>(Tabela32[[#This Row],[Różnica ]]/Tabela32[[#This Row],[Liczba Żubrów]])*100%</f>
+        <v>6.684594698424895E-2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
 </file>
</xml_diff>